<commit_message>
update quote e velocità approccio prelevamento ferriti
</commit_message>
<xml_diff>
--- a/calcolo posizione ferriti.xlsx
+++ b/calcolo posizione ferriti.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BMTec_HP_01\Documents\Denso\Denso-Robot-Prg-Comelit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D6DE0B-59A8-48E3-9CCC-E792FC5AB287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3F80C9-78FC-4198-881C-D238BA66B7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{797D2BC8-58BE-49C8-B377-261DF778AF65}"/>
   </bookViews>
@@ -19,6 +19,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -55,12 +63,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -90,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -99,6 +113,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -415,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEFA528-0B1D-4083-A0AD-47884D379F0C}">
-  <dimension ref="F1:AH29"/>
+  <dimension ref="F1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,10 +495,10 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>5</v>
       </c>
       <c r="J5" s="1">
@@ -494,10 +511,10 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>20</v>
       </c>
       <c r="J6" s="1">
@@ -530,10 +547,10 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>19</v>
       </c>
       <c r="J9" s="1">

</xml_diff>